<commit_message>
Lista pagina, falta agregar pagos especificos por estudiante
</commit_message>
<xml_diff>
--- a/otherfiles/PlanillaPaola.xlsx
+++ b/otherfiles/PlanillaPaola.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Git\Orkesta\otherfiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{300B9EB6-B4E9-4E51-8B80-EB5A7B515373}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="21315" windowHeight="10035"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="21315" windowHeight="10035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -81,9 +87,6 @@
     <t>Castellani Sofia</t>
   </si>
   <si>
-    <t>Coro</t>
-  </si>
-  <si>
     <t>Muñoz, Elishama/Muñoz, Eliab/Muñoz, Eliabris</t>
   </si>
   <si>
@@ -375,9 +378,6 @@
     <t>Victor Cordova/Victoria Cordova/Elinel Arciniegas</t>
   </si>
   <si>
-    <t>Inicial/Inicial/Coro Padres</t>
-  </si>
-  <si>
     <t>38459874</t>
   </si>
   <si>
@@ -520,14 +520,20 @@
   </si>
   <si>
     <t>58764384</t>
+  </si>
+  <si>
+    <t>Inicial/Inicial/Coro de Padres</t>
+  </si>
+  <si>
+    <t>Coro de Padres</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_ &quot;Bs. F&quot;\ * #,##0.00_ ;_ &quot;Bs. F&quot;\ * \-#,##0.00_ ;_ &quot;Bs. F&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ &quot;Bs. F&quot;\ * #,##0.00_ ;_ &quot;Bs. F&quot;\ * \-#,##0.00_ ;_ &quot;Bs. F&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -581,7 +587,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -596,23 +602,94 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="FFFFFF"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="3C3C3C"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -647,7 +724,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -680,9 +757,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -715,6 +809,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -890,21 +1001,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="G94" sqref="G94"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.42578125" customWidth="1"/>
     <col min="2" max="2" width="31.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="6" max="6" width="19.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1009,10 +1120,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -1030,7 +1141,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>18</v>
@@ -1081,7 +1192,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1105,7 +1216,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>21</v>
+        <v>167</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
@@ -1126,7 +1237,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>19</v>
@@ -1150,13 +1261,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>10</v>
@@ -1174,10 +1285,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
@@ -1198,10 +1309,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>5</v>
@@ -1222,10 +1333,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>5</v>
@@ -1246,13 +1357,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>10</v>
@@ -1270,7 +1381,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>5</v>
@@ -1294,10 +1405,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
@@ -1318,13 +1429,13 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>5</v>
@@ -1342,13 +1453,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>5</v>
@@ -1366,7 +1477,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>5</v>
@@ -1390,7 +1501,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>5</v>
@@ -1414,10 +1525,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>5</v>
@@ -1438,10 +1549,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>5</v>
@@ -1462,13 +1573,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>5</v>
@@ -1486,7 +1597,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>5</v>
@@ -1501,7 +1612,7 @@
         <v>43266</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G25" s="3">
         <v>500000</v>
@@ -1510,7 +1621,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>5</v>
@@ -1525,7 +1636,7 @@
         <v>43271</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G26" s="3">
         <v>200000</v>
@@ -1534,10 +1645,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>5</v>
@@ -1558,10 +1669,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>5</v>
@@ -1573,7 +1684,7 @@
         <v>5</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G28" s="3">
         <v>200000</v>
@@ -1582,13 +1693,13 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>5</v>
@@ -1597,7 +1708,7 @@
         <v>43272</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G29" s="3">
         <v>200000</v>
@@ -1606,16 +1717,16 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="E30" s="4">
         <v>43272</v>
@@ -1639,13 +1750,13 @@
         <v>5</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E31" s="4">
         <v>43272</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G31" s="3">
         <v>500000</v>
@@ -1654,22 +1765,22 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E32" s="4">
         <v>43271</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G32" s="3">
         <v>200000</v>
@@ -1678,13 +1789,13 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>10</v>
@@ -1693,7 +1804,7 @@
         <v>43272</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G33" s="3">
         <v>200000</v>
@@ -1702,7 +1813,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>5</v>
@@ -1717,7 +1828,7 @@
         <v>43272</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G34" s="3">
         <v>1000000</v>
@@ -1726,22 +1837,22 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="E35" s="4">
         <v>43270</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G35" s="3">
         <v>200000</v>
@@ -1750,22 +1861,22 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="E36" s="4">
         <v>43272</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G36" s="3">
         <v>200000</v>
@@ -1774,22 +1885,22 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="G37" s="3">
         <v>200000</v>
@@ -1798,10 +1909,10 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>5</v>
@@ -1813,7 +1924,7 @@
         <v>43259</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G38" s="3">
         <v>1000000</v>
@@ -1822,10 +1933,10 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>5</v>
@@ -1846,10 +1957,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>5</v>
@@ -1861,7 +1972,7 @@
         <v>43271</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G40" s="3">
         <v>200000</v>
@@ -1869,10 +1980,10 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>5</v>
@@ -1884,7 +1995,7 @@
         <v>43271</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G41" s="3">
         <v>500000</v>
@@ -1892,7 +2003,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>5</v>
@@ -1901,13 +2012,13 @@
         <v>5</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E42" s="4">
         <v>43270</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G42" s="3">
         <v>200000</v>
@@ -1915,10 +2026,10 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>5</v>
@@ -1930,7 +2041,7 @@
         <v>43251</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G43" s="3">
         <v>200000</v>
@@ -1938,22 +2049,22 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E44" s="4">
         <v>43264</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G44" s="3">
         <v>220000</v>
@@ -1961,22 +2072,22 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E45" s="4">
         <v>43174</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G45" s="3">
         <v>10000</v>
@@ -1984,10 +2095,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>5</v>
@@ -1999,7 +2110,7 @@
         <v>43270</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G46" s="3">
         <v>600000</v>
@@ -2007,10 +2118,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>5</v>
@@ -2022,7 +2133,7 @@
         <v>43270</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G47" s="3">
         <v>400000</v>
@@ -2030,22 +2141,22 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E48" s="4">
         <v>43258</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G48" s="3">
         <v>800000</v>
@@ -2053,22 +2164,22 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E49" s="4">
         <v>43258</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G49" s="3">
         <v>500000</v>
@@ -2076,22 +2187,22 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E50" s="4">
         <v>43258</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G50" s="3">
         <v>200000</v>
@@ -2099,10 +2210,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>5</v>
@@ -2122,10 +2233,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>5</v>
@@ -2137,7 +2248,7 @@
         <v>43270</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G52" s="3">
         <v>200000</v>
@@ -2145,10 +2256,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>5</v>
@@ -2160,7 +2271,7 @@
         <v>43269</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G53" s="3">
         <v>1000000</v>
@@ -2168,10 +2279,10 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>5</v>
@@ -2183,7 +2294,7 @@
         <v>43258</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G54" s="3">
         <v>200000</v>
@@ -2191,10 +2302,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>5</v>
@@ -2206,7 +2317,7 @@
         <v>43266</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G55" s="3">
         <v>200000</v>
@@ -2214,10 +2325,10 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>5</v>
@@ -2229,7 +2340,7 @@
         <v>43269</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G56" s="3">
         <v>200000</v>
@@ -2237,10 +2348,10 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>5</v>
@@ -2252,7 +2363,7 @@
         <v>43269</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G57" s="3">
         <v>200000</v>
@@ -2260,22 +2371,22 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E58" s="4">
         <v>43259</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G58" s="3">
         <v>1000000</v>
@@ -2283,10 +2394,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>5</v>
@@ -2298,7 +2409,7 @@
         <v>43258</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G59" s="3">
         <v>1000000</v>
@@ -2306,10 +2417,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>5</v>
@@ -2321,7 +2432,7 @@
         <v>43259</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G60" s="3">
         <v>600000</v>
@@ -2329,22 +2440,22 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>119</v>
+        <v>166</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E61" s="4">
         <v>43256</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G61" s="3">
         <v>800000</v>
@@ -2352,22 +2463,22 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="D62" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E62" s="4">
         <v>43235</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G62" s="3">
         <v>200000</v>
@@ -2375,22 +2486,22 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="D63" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E63" s="4">
         <v>43245</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G63" s="3">
         <v>200000</v>
@@ -2398,10 +2509,10 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>5</v>
@@ -2421,10 +2532,10 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>5</v>
@@ -2436,7 +2547,7 @@
         <v>5</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G65" s="3">
         <v>200000</v>
@@ -2444,10 +2555,10 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>5</v>
@@ -2459,7 +2570,7 @@
         <v>5</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G66" s="3">
         <v>400000</v>
@@ -2467,22 +2578,22 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E67" s="4">
         <v>43081</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G67" s="3">
         <v>20000</v>
@@ -2490,22 +2601,22 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E68" s="4">
         <v>43123</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G68" s="3">
         <v>40000</v>
@@ -2513,22 +2624,22 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E69" s="4">
         <v>43123</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G69" s="3">
         <v>100000</v>
@@ -2536,22 +2647,22 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E70" s="4">
         <v>43171</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G70" s="3">
         <v>50000</v>
@@ -2559,22 +2670,22 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E71" s="4">
         <v>43208</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G71" s="3">
         <v>200000</v>
@@ -2582,22 +2693,22 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E72" s="4">
         <v>43236</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G72" s="3">
         <v>350000</v>
@@ -2605,22 +2716,22 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E73" s="4">
         <v>43194</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G73" s="3">
         <v>150000</v>
@@ -2628,7 +2739,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>5</v>
@@ -2643,7 +2754,7 @@
         <v>5</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G74" s="3">
         <v>2000000</v>
@@ -2651,13 +2762,13 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>6</v>
@@ -2666,7 +2777,7 @@
         <v>43257</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G75" s="3">
         <v>200000</v>
@@ -2674,10 +2785,10 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>5</v>
@@ -2689,7 +2800,7 @@
         <v>43259</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G76" s="3">
         <v>400000</v>
@@ -2697,10 +2808,10 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>5</v>
@@ -2720,10 +2831,10 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>5</v>
@@ -2735,7 +2846,7 @@
         <v>43242</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G78" s="3">
         <v>200000</v>
@@ -2743,10 +2854,10 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>5</v>
@@ -2758,7 +2869,7 @@
         <v>43242</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G79" s="3">
         <v>500000</v>
@@ -2766,10 +2877,10 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>5</v>
@@ -2781,7 +2892,7 @@
         <v>43258</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G80" s="3">
         <v>570000</v>
@@ -2789,10 +2900,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>5</v>
@@ -2804,7 +2915,7 @@
         <v>43223</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G81" s="3">
         <v>40000</v>
@@ -2812,10 +2923,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>5</v>
@@ -2827,7 +2938,7 @@
         <v>43149</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G82" s="3">
         <v>30000</v>
@@ -2835,10 +2946,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>5</v>
@@ -2850,7 +2961,7 @@
         <v>43081</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G83" s="3">
         <v>15000</v>
@@ -2858,7 +2969,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>5</v>
@@ -2870,7 +2981,7 @@
         <v>6</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F84" s="5" t="s">
         <v>5</v>
@@ -2881,7 +2992,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>5</v>
@@ -2896,7 +3007,7 @@
         <v>43259</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G85" s="3">
         <v>200000</v>
@@ -2904,22 +3015,22 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E86" s="4">
         <v>43259</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G86" s="3">
         <v>1000000</v>
@@ -2927,22 +3038,22 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E87" s="4">
         <v>43259</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G87" s="3">
         <v>1100000</v>
@@ -2965,7 +3076,7 @@
         <v>43259</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G88" s="3">
         <v>700000</v>
@@ -2973,10 +3084,10 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>5</v>
@@ -2988,7 +3099,7 @@
         <v>43091</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G89" s="3">
         <v>12500</v>
@@ -2996,10 +3107,10 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>5</v>
@@ -3011,7 +3122,7 @@
         <v>42764</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G90" s="3">
         <v>10000</v>
@@ -3019,10 +3130,10 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>5</v>
@@ -3034,7 +3145,7 @@
         <v>43160</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G91" s="3">
         <v>10000</v>
@@ -3042,10 +3153,10 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>5</v>
@@ -3057,7 +3168,7 @@
         <v>43175</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G92" s="3">
         <v>10000</v>
@@ -3065,10 +3176,10 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>5</v>
@@ -3080,7 +3191,7 @@
         <v>43256</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G93" s="3">
         <v>50000</v>
@@ -3282,24 +3393,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>